<commit_message>
Adding metrics calculation to code for temporal series
</commit_message>
<xml_diff>
--- a/raw_data/raw_excel/Crinita_Port_Selva_2017-set 2019_ordenatSC.xlsx
+++ b/raw_data/raw_excel/Crinita_Port_Selva_2017-set 2019_ordenatSC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/avipo_dtu_dk/Documents/Skrivebord/Postdoc/Projects/Fenology_cysto/raw_data/raw_excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avipo\OneDrive - Danmarks Tekniske Universitet\Skrivebord\Postdoc\Projects\Fenology_cysto\raw_data\raw_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_B7B6413C8F3E4FADC1E22088B839D82B64B80C90" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217AE333-7DC6-45F8-8342-438C38B67302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-9945" windowWidth="14400" windowHeight="15600" firstSheet="17" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estructura talles" sheetId="5" r:id="rId1"/>
@@ -4856,8 +4856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J153"/>
   <sheetViews>
-    <sheetView topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="G149" sqref="G149:H153"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8093,8 +8093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J143"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="G139" sqref="G139:H143"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39:E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10890,7 +10890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I260"/>
   <sheetViews>
-    <sheetView topLeftCell="A229" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E256" sqref="E256:F260"/>
     </sheetView>
   </sheetViews>
@@ -15759,7 +15759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J157"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="F158" sqref="F158"/>
     </sheetView>
   </sheetViews>
@@ -18911,7 +18911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J196"/>
   <sheetViews>
-    <sheetView topLeftCell="A165" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="E192" sqref="E192:F196"/>
     </sheetView>
   </sheetViews>
@@ -22643,7 +22643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J190"/>
   <sheetViews>
-    <sheetView topLeftCell="A137" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="E164" sqref="E164:F168"/>
     </sheetView>
   </sheetViews>
@@ -28643,8 +28643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:L190"/>
   <sheetViews>
-    <sheetView topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="E134" sqref="E134:F138"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32044,7 +32044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:L193"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E128" sqref="E128:F132"/>
     </sheetView>
   </sheetViews>
@@ -35244,7 +35244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:L284"/>
   <sheetViews>
-    <sheetView topLeftCell="A251" workbookViewId="0">
+    <sheetView topLeftCell="A158" workbookViewId="0">
       <selection activeCell="F283" sqref="F283"/>
     </sheetView>
   </sheetViews>
@@ -44641,8 +44641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:L280"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="E146" sqref="E146:F150"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53267,10 +53267,10 @@
   <dimension ref="A1:M409"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B386" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B389" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P390" sqref="P390"/>
+      <selection pane="bottomRight" activeCell="H402" sqref="H402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -67574,7 +67574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView topLeftCell="A177" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:E194"/>
     </sheetView>
   </sheetViews>
@@ -71036,8 +71036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q167"/>
   <sheetViews>
-    <sheetView topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -74499,8 +74499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="E146" sqref="E146"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="G96" sqref="G96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -78790,8 +78790,8 @@
   <dimension ref="A1:J195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G191" sqref="G191:H195"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -82990,7 +82990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J136"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
+    <sheetView topLeftCell="A109" workbookViewId="0">
       <selection activeCell="G132" sqref="G132:H136"/>
     </sheetView>
   </sheetViews>
@@ -85554,7 +85554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
@@ -87628,7 +87628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:J155"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
+    <sheetView topLeftCell="A118" workbookViewId="0">
       <selection activeCell="G151" sqref="G151:H155"/>
     </sheetView>
   </sheetViews>

</xml_diff>